<commit_message>
Updated control definition, added high WC, high WHR and BMI categories
</commit_message>
<xml_diff>
--- a/data/NFHS Cascade Variable List.xlsx
+++ b/data/NFHS Cascade Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A085EBA7-92C0-41D2-B7DF-48A765DD37D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB52040C-BE02-4C7E-B198-AE3FE2CB6438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="553">
   <si>
     <t>label</t>
   </si>
@@ -1274,9 +1274,6 @@
     <t>sh47</t>
   </si>
   <si>
-    <t>religion of hh</t>
-  </si>
-  <si>
     <t>caste of hh</t>
   </si>
   <si>
@@ -1497,6 +1494,192 @@
   </si>
   <si>
     <t>sh25</t>
+  </si>
+  <si>
+    <t>new_var</t>
+  </si>
+  <si>
+    <t>state2</t>
+  </si>
+  <si>
+    <t>residence2</t>
+  </si>
+  <si>
+    <t>linenumber</t>
+  </si>
+  <si>
+    <t>sampleweight</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>month_interview</t>
+  </si>
+  <si>
+    <t>year_interview</t>
+  </si>
+  <si>
+    <t>day_interview</t>
+  </si>
+  <si>
+    <t>date_interview_cmc</t>
+  </si>
+  <si>
+    <t>date_interview_cdc</t>
+  </si>
+  <si>
+    <t>nmembers</t>
+  </si>
+  <si>
+    <t>eduyr</t>
+  </si>
+  <si>
+    <t>marital</t>
+  </si>
+  <si>
+    <t>wealthq</t>
+  </si>
+  <si>
+    <t>wealths</t>
+  </si>
+  <si>
+    <t>wealths_ur</t>
+  </si>
+  <si>
+    <t>wealthq_ur</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>result_anthro</t>
+  </si>
+  <si>
+    <t>bmi</t>
+  </si>
+  <si>
+    <t>waistcircumference</t>
+  </si>
+  <si>
+    <t>hipcircumference</t>
+  </si>
+  <si>
+    <t>wc_refusal</t>
+  </si>
+  <si>
+    <t>hc_refusal</t>
+  </si>
+  <si>
+    <t>hb_consent</t>
+  </si>
+  <si>
+    <t>hb</t>
+  </si>
+  <si>
+    <t>pregnant</t>
+  </si>
+  <si>
+    <t>hb_result</t>
+  </si>
+  <si>
+    <t>hb_adjusted</t>
+  </si>
+  <si>
+    <t>anemia</t>
+  </si>
+  <si>
+    <t>screened_bp</t>
+  </si>
+  <si>
+    <t>diagnosed_bp</t>
+  </si>
+  <si>
+    <t>medication_bp</t>
+  </si>
+  <si>
+    <t>glucose</t>
+  </si>
+  <si>
+    <t>screened_dm</t>
+  </si>
+  <si>
+    <t>diagnosed_dm</t>
+  </si>
+  <si>
+    <t>medication_dm</t>
+  </si>
+  <si>
+    <t>bp_30min_eaten</t>
+  </si>
+  <si>
+    <t>bp_30min_coffee</t>
+  </si>
+  <si>
+    <t>bp_30min_smoke</t>
+  </si>
+  <si>
+    <t>smokecount</t>
+  </si>
+  <si>
+    <t>bp_30min_other</t>
+  </si>
+  <si>
+    <t>bp_armcircumference</t>
+  </si>
+  <si>
+    <t>bp_cuffsize</t>
+  </si>
+  <si>
+    <t>bp1_time</t>
+  </si>
+  <si>
+    <t>sbp1</t>
+  </si>
+  <si>
+    <t>dbp1</t>
+  </si>
+  <si>
+    <t>bp2_time</t>
+  </si>
+  <si>
+    <t>sbp2</t>
+  </si>
+  <si>
+    <t>dbp2</t>
+  </si>
+  <si>
+    <t>bp3_time</t>
+  </si>
+  <si>
+    <t>sbp3</t>
+  </si>
+  <si>
+    <t>dbp3</t>
+  </si>
+  <si>
+    <t>lastate</t>
+  </si>
+  <si>
+    <t>lastdrank</t>
+  </si>
+  <si>
+    <t>glucose_time</t>
+  </si>
+  <si>
+    <t>nchildren</t>
+  </si>
+  <si>
+    <t>caseid</t>
+  </si>
+  <si>
+    <t>smokecurr</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1561,6 +1744,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1841,1643 +2025,1859 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BB052-C333-4DDF-AF33-13FC35516278}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.26953125" customWidth="1"/>
-    <col min="4" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>308</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>167</v>
       </c>
       <c r="E2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
       <c r="B3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C3" t="s">
         <v>309</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>322</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
+        <v>551</v>
+      </c>
+      <c r="D5" t="s">
         <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>162</v>
       </c>
       <c r="E5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>171</v>
       </c>
       <c r="B6" t="s">
+        <v>494</v>
+      </c>
+      <c r="C6" t="s">
         <v>307</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>306</v>
-      </c>
-      <c r="D6" t="s">
-        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>51</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
       </c>
       <c r="E7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
       <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>113</v>
-      </c>
-      <c r="D8" t="s">
-        <v>169</v>
       </c>
       <c r="E8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>57</v>
       </c>
       <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>114</v>
-      </c>
-      <c r="D9" t="s">
-        <v>170</v>
       </c>
       <c r="E9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>115</v>
-      </c>
-      <c r="D10" t="s">
-        <v>164</v>
       </c>
       <c r="E10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>166</v>
       </c>
       <c r="B11" t="s">
+        <v>495</v>
+      </c>
+      <c r="C11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>116</v>
-      </c>
-      <c r="D11" t="s">
-        <v>165</v>
       </c>
       <c r="E11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>481</v>
+      </c>
+      <c r="B12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E12" t="s">
+        <v>475</v>
+      </c>
+      <c r="F12" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>482</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B13" t="s">
+        <v>498</v>
+      </c>
+      <c r="E13" t="s">
         <v>476</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F13" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>486</v>
+      </c>
+      <c r="B14" t="s">
+        <v>499</v>
+      </c>
+      <c r="E14" t="s">
+        <v>487</v>
+      </c>
+      <c r="F14" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>483</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B15" t="s">
+        <v>500</v>
+      </c>
+      <c r="E15" t="s">
         <v>477</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F15" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>487</v>
-      </c>
-      <c r="D14" t="s">
-        <v>488</v>
-      </c>
-      <c r="E14" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>484</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
+        <v>501</v>
+      </c>
+      <c r="E16" t="s">
         <v>478</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F16" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>485</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B17" t="s">
+        <v>502</v>
+      </c>
+      <c r="E17" t="s">
         <v>479</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F17" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>481</v>
-      </c>
-      <c r="D17" t="s">
-        <v>480</v>
-      </c>
-      <c r="E17" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>415</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" t="s">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>417</v>
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>416</v>
+        <v>118</v>
       </c>
       <c r="E20" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>417</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+      <c r="D21" t="s">
+        <v>311</v>
+      </c>
+      <c r="E21" t="s">
+        <v>418</v>
+      </c>
+      <c r="F21" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>418</v>
+        <v>313</v>
+      </c>
+      <c r="B22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C22" t="s">
+        <v>315</v>
       </c>
       <c r="D22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B23" t="s">
+        <v>503</v>
+      </c>
+      <c r="C23" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" t="s">
+        <v>318</v>
+      </c>
+      <c r="E23" t="s">
+        <v>421</v>
+      </c>
+      <c r="F23" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>313</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>420</v>
+      </c>
+      <c r="F24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" t="s">
         <v>419</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F25" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>312</v>
-      </c>
-      <c r="C23" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>313</v>
-      </c>
-      <c r="B24" t="s">
-        <v>315</v>
-      </c>
-      <c r="C24" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>316</v>
-      </c>
-      <c r="B25" t="s">
-        <v>317</v>
-      </c>
-      <c r="C25" t="s">
-        <v>318</v>
-      </c>
-      <c r="D25" t="s">
-        <v>422</v>
-      </c>
-      <c r="E25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>493</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" t="s">
+        <v>504</v>
+      </c>
+      <c r="C27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D27" t="s">
+        <v>297</v>
+      </c>
+      <c r="E27" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" t="s">
-        <v>421</v>
-      </c>
-      <c r="E26" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" t="s">
-        <v>420</v>
-      </c>
-      <c r="E27" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>125</v>
+        <v>295</v>
       </c>
       <c r="C28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+      <c r="D28" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>294</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>292</v>
+        <v>505</v>
       </c>
       <c r="C29" t="s">
-        <v>297</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" t="s">
         <v>424</v>
       </c>
-      <c r="E29" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>295</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>506</v>
       </c>
       <c r="C30" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" t="s">
+        <v>425</v>
+      </c>
+      <c r="F30" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>426</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" t="s">
-        <v>425</v>
+        <v>508</v>
       </c>
       <c r="E31" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>427</v>
+      </c>
+      <c r="F31" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>429</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" t="s">
-        <v>426</v>
+        <v>507</v>
       </c>
       <c r="E32" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>428</v>
+      </c>
+      <c r="F32" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>427</v>
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>428</v>
-      </c>
-      <c r="E33" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>341</v>
+      </c>
+      <c r="D35" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>343</v>
+      </c>
+      <c r="D38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>324</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>358</v>
+      </c>
+      <c r="C41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>325</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>328</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>360</v>
+      </c>
+      <c r="C44" t="s">
+        <v>334</v>
+      </c>
+      <c r="D44" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>327</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>329</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>330</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" t="s">
+        <v>509</v>
+      </c>
+      <c r="C48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D48" t="s">
+        <v>239</v>
+      </c>
+      <c r="E48" t="s">
+        <v>485</v>
+      </c>
+      <c r="F48" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" t="s">
+        <v>250</v>
+      </c>
+      <c r="D49" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>231</v>
+      </c>
+      <c r="C50" t="s">
+        <v>251</v>
+      </c>
+      <c r="D50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>232</v>
+      </c>
+      <c r="C51" t="s">
+        <v>252</v>
+      </c>
+      <c r="D51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" t="s">
+        <v>253</v>
+      </c>
+      <c r="D52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" t="s">
+        <v>255</v>
+      </c>
+      <c r="D54" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" t="s">
+        <v>256</v>
+      </c>
+      <c r="D55" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>175</v>
+      </c>
+      <c r="C58" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" t="s">
+        <v>510</v>
+      </c>
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+      <c r="E60" t="s">
         <v>430</v>
       </c>
-      <c r="D34" t="s">
-        <v>429</v>
-      </c>
-      <c r="E34" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" t="s">
-        <v>341</v>
-      </c>
-      <c r="C37" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>343</v>
-      </c>
-      <c r="C40" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" t="s">
-        <v>324</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>358</v>
-      </c>
-      <c r="B43" t="s">
-        <v>326</v>
-      </c>
-      <c r="C43" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" t="s">
-        <v>325</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" t="s">
-        <v>328</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>360</v>
-      </c>
-      <c r="B46" t="s">
-        <v>334</v>
-      </c>
-      <c r="C46" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" t="s">
-        <v>327</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
-        <v>329</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" t="s">
-        <v>330</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>229</v>
-      </c>
-      <c r="B50" t="s">
-        <v>249</v>
-      </c>
-      <c r="C50" t="s">
-        <v>239</v>
-      </c>
-      <c r="D50" t="s">
-        <v>486</v>
-      </c>
-      <c r="E50" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>230</v>
-      </c>
-      <c r="B51" t="s">
-        <v>250</v>
-      </c>
-      <c r="C51" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52" t="s">
-        <v>251</v>
-      </c>
-      <c r="C52" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B53" t="s">
-        <v>252</v>
-      </c>
-      <c r="C53" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>233</v>
-      </c>
-      <c r="B54" t="s">
-        <v>253</v>
-      </c>
-      <c r="C54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>234</v>
-      </c>
-      <c r="B55" t="s">
-        <v>254</v>
-      </c>
-      <c r="C55" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>235</v>
-      </c>
-      <c r="B56" t="s">
-        <v>255</v>
-      </c>
-      <c r="C56" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>236</v>
-      </c>
-      <c r="B57" t="s">
-        <v>256</v>
-      </c>
-      <c r="C57" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>237</v>
-      </c>
-      <c r="B58" t="s">
-        <v>257</v>
-      </c>
-      <c r="C58" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>238</v>
-      </c>
-      <c r="B59" t="s">
-        <v>258</v>
-      </c>
-      <c r="C59" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>511</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+      <c r="E61" t="s">
+        <v>431</v>
+      </c>
+      <c r="F61" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>281</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
-      </c>
-      <c r="D62" t="s">
-        <v>431</v>
+        <v>512</v>
       </c>
       <c r="E62" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>432</v>
+      </c>
+      <c r="F62" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D63" t="s">
-        <v>432</v>
+        <v>513</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+      <c r="F63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>281</v>
+        <v>388</v>
+      </c>
+      <c r="B64" t="s">
+        <v>514</v>
+      </c>
+      <c r="C64" t="s">
+        <v>389</v>
       </c>
       <c r="D64" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
       <c r="E64" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>390</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>515</v>
+      </c>
+      <c r="C65" t="s">
+        <v>391</v>
       </c>
       <c r="D65" t="s">
-        <v>434</v>
+        <v>404</v>
       </c>
       <c r="E65" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+        <v>435</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>388</v>
+        <v>436</v>
       </c>
       <c r="B66" t="s">
-        <v>389</v>
-      </c>
-      <c r="C66" t="s">
-        <v>403</v>
-      </c>
-      <c r="D66" t="s">
-        <v>435</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+        <v>516</v>
+      </c>
+      <c r="E66" t="s">
+        <v>437</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>390</v>
+        <v>438</v>
       </c>
       <c r="B67" t="s">
-        <v>391</v>
-      </c>
-      <c r="C67" t="s">
-        <v>404</v>
-      </c>
-      <c r="D67" t="s">
-        <v>436</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+        <v>517</v>
+      </c>
+      <c r="E67" t="s">
+        <v>474</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>437</v>
-      </c>
-      <c r="D68" t="s">
-        <v>438</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+      <c r="B68" t="s">
+        <v>518</v>
+      </c>
+      <c r="C68" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" t="s">
+        <v>441</v>
+      </c>
+      <c r="F68" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>184</v>
+      </c>
+      <c r="B69" t="s">
+        <v>519</v>
+      </c>
+      <c r="C69" t="s">
+        <v>183</v>
+      </c>
+      <c r="E69" t="s">
+        <v>442</v>
+      </c>
+      <c r="F69" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>185</v>
+      </c>
+      <c r="B70" t="s">
+        <v>520</v>
+      </c>
+      <c r="C70" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>186</v>
+      </c>
+      <c r="B71" t="s">
+        <v>521</v>
+      </c>
+      <c r="C71" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" t="s">
+        <v>444</v>
+      </c>
+      <c r="F71" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" t="s">
+        <v>522</v>
+      </c>
+      <c r="C72" t="s">
+        <v>190</v>
+      </c>
+      <c r="E72" t="s">
+        <v>445</v>
+      </c>
+      <c r="F72" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>447</v>
+      </c>
+      <c r="B73" t="s">
+        <v>523</v>
+      </c>
+      <c r="E73" t="s">
+        <v>446</v>
+      </c>
+      <c r="F73" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>272</v>
+      </c>
+      <c r="B75" t="s">
+        <v>496</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D75" t="s">
+        <v>347</v>
+      </c>
+      <c r="E75" t="s">
+        <v>488</v>
+      </c>
+      <c r="F75" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>489</v>
+      </c>
+      <c r="B76" t="s">
+        <v>552</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="E76" t="s">
+        <v>490</v>
+      </c>
+      <c r="F76" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>270</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D77" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>191</v>
+      </c>
+      <c r="C78" t="s">
+        <v>210</v>
+      </c>
+      <c r="D78" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>192</v>
+      </c>
+      <c r="C79" t="s">
+        <v>211</v>
+      </c>
+      <c r="D79" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81" t="s">
+        <v>213</v>
+      </c>
+      <c r="D81" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>195</v>
+      </c>
+      <c r="C82" t="s">
+        <v>214</v>
+      </c>
+      <c r="D82" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="s">
+        <v>215</v>
+      </c>
+      <c r="D83" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" t="s">
+        <v>216</v>
+      </c>
+      <c r="D84" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" t="s">
+        <v>217</v>
+      </c>
+      <c r="D85" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>199</v>
+      </c>
+      <c r="C86" t="s">
+        <v>218</v>
+      </c>
+      <c r="D86" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>201</v>
+      </c>
+      <c r="C88" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>204</v>
+      </c>
+      <c r="C91" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>205</v>
+      </c>
+      <c r="C92" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>206</v>
+      </c>
+      <c r="C93" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>207</v>
+      </c>
+      <c r="C94" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>208</v>
+      </c>
+      <c r="C95" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>209</v>
+      </c>
+      <c r="C96" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C98" t="s">
+        <v>97</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="C99" t="s">
+        <v>357</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>333</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="C100" t="s">
+        <v>361</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>400</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="C101" t="s">
+        <v>401</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>399</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="C103" t="s">
+        <v>378</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="C104" t="s">
+        <v>349</v>
+      </c>
+      <c r="D104" t="s">
+        <v>405</v>
+      </c>
+      <c r="E104" t="s">
+        <v>449</v>
+      </c>
+      <c r="F104" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="C105" t="s">
+        <v>350</v>
+      </c>
+      <c r="D105" t="s">
+        <v>406</v>
+      </c>
+      <c r="E105" t="s">
+        <v>450</v>
+      </c>
+      <c r="F105" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="C106" t="s">
+        <v>351</v>
+      </c>
+      <c r="D106" t="s">
+        <v>407</v>
+      </c>
+      <c r="E106" t="s">
+        <v>451</v>
+      </c>
+      <c r="F106" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>439</v>
       </c>
-      <c r="D69" t="s">
-        <v>475</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" t="s">
-        <v>182</v>
-      </c>
-      <c r="D70" t="s">
-        <v>442</v>
-      </c>
-      <c r="E70" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>184</v>
-      </c>
-      <c r="B71" t="s">
-        <v>183</v>
-      </c>
-      <c r="D71" t="s">
-        <v>443</v>
-      </c>
-      <c r="E71" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>185</v>
-      </c>
-      <c r="B72" t="s">
-        <v>188</v>
-      </c>
-      <c r="D72" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>186</v>
-      </c>
-      <c r="B73" t="s">
-        <v>189</v>
-      </c>
-      <c r="D73" t="s">
-        <v>445</v>
-      </c>
-      <c r="E73" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B74" t="s">
-        <v>190</v>
-      </c>
-      <c r="D74" t="s">
-        <v>446</v>
-      </c>
-      <c r="E74" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>448</v>
-      </c>
-      <c r="D75" t="s">
-        <v>447</v>
-      </c>
-      <c r="E75" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>272</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C77" t="s">
-        <v>347</v>
-      </c>
-      <c r="D77" t="s">
-        <v>489</v>
-      </c>
-      <c r="E77" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>490</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="D78" t="s">
-        <v>491</v>
-      </c>
-      <c r="E78" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>270</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C79" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>191</v>
-      </c>
-      <c r="B80" t="s">
-        <v>210</v>
-      </c>
-      <c r="C80" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>192</v>
-      </c>
-      <c r="B81" t="s">
-        <v>211</v>
-      </c>
-      <c r="C81" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>193</v>
-      </c>
-      <c r="B82" t="s">
-        <v>212</v>
-      </c>
-      <c r="C82" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>194</v>
-      </c>
-      <c r="B83" t="s">
-        <v>213</v>
-      </c>
-      <c r="C83" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>195</v>
-      </c>
-      <c r="B84" t="s">
-        <v>214</v>
-      </c>
-      <c r="C84" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>196</v>
-      </c>
-      <c r="B85" t="s">
-        <v>215</v>
-      </c>
-      <c r="C85" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>197</v>
-      </c>
-      <c r="B86" t="s">
-        <v>216</v>
-      </c>
-      <c r="C86" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>198</v>
-      </c>
-      <c r="B87" t="s">
-        <v>217</v>
-      </c>
-      <c r="C87" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>199</v>
-      </c>
-      <c r="B88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" t="s">
-        <v>219</v>
-      </c>
-      <c r="C89" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>201</v>
-      </c>
-      <c r="B90" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>202</v>
-      </c>
-      <c r="B91" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>203</v>
-      </c>
-      <c r="B92" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>204</v>
-      </c>
-      <c r="B93" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>205</v>
-      </c>
-      <c r="B94" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>206</v>
-      </c>
-      <c r="B95" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>207</v>
-      </c>
-      <c r="B96" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>208</v>
-      </c>
-      <c r="B97" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>209</v>
-      </c>
-      <c r="B98" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>25</v>
-      </c>
-      <c r="B100" t="s">
-        <v>97</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" t="s">
-        <v>357</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>333</v>
-      </c>
-      <c r="B102" t="s">
-        <v>361</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>400</v>
-      </c>
-      <c r="B103" t="s">
-        <v>401</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>399</v>
-      </c>
-      <c r="B105" t="s">
-        <v>378</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>15</v>
-      </c>
-      <c r="B106" t="s">
-        <v>349</v>
-      </c>
-      <c r="C106" t="s">
-        <v>405</v>
-      </c>
-      <c r="D106" t="s">
-        <v>450</v>
-      </c>
-      <c r="E106" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>16</v>
-      </c>
-      <c r="B107" t="s">
-        <v>350</v>
-      </c>
-      <c r="C107" t="s">
-        <v>406</v>
-      </c>
-      <c r="D107" t="s">
-        <v>451</v>
+      <c r="B107" s="7" t="s">
+        <v>534</v>
       </c>
       <c r="E107" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+      <c r="F107" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>17</v>
-      </c>
-      <c r="B108" t="s">
-        <v>351</v>
+        <v>18</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>535</v>
       </c>
       <c r="C108" t="s">
-        <v>407</v>
+        <v>352</v>
       </c>
       <c r="D108" t="s">
-        <v>452</v>
+        <v>408</v>
       </c>
       <c r="E108" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F108" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>440</v>
+        <v>19</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="C109" t="s">
+        <v>353</v>
       </c>
       <c r="D109" t="s">
-        <v>441</v>
+        <v>392</v>
       </c>
       <c r="E109" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+        <v>453</v>
+      </c>
+      <c r="F109" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>18</v>
-      </c>
-      <c r="B110" t="s">
-        <v>352</v>
+        <v>20</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>537</v>
       </c>
       <c r="C110" t="s">
-        <v>408</v>
+        <v>354</v>
       </c>
       <c r="D110" t="s">
-        <v>453</v>
+        <v>393</v>
       </c>
       <c r="E110" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+        <v>454</v>
+      </c>
+      <c r="F110" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>19</v>
-      </c>
-      <c r="B111" t="s">
-        <v>353</v>
+        <v>366</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>538</v>
       </c>
       <c r="C111" t="s">
-        <v>392</v>
+        <v>95</v>
       </c>
       <c r="D111" t="s">
-        <v>454</v>
+        <v>139</v>
       </c>
       <c r="E111" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+      <c r="F111" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>20</v>
-      </c>
-      <c r="B112" t="s">
-        <v>354</v>
+        <v>23</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>539</v>
       </c>
       <c r="C112" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
       <c r="D112" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
       <c r="E112" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+        <v>456</v>
+      </c>
+      <c r="F112" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>366</v>
-      </c>
-      <c r="B113" t="s">
-        <v>95</v>
+        <v>24</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>540</v>
       </c>
       <c r="C113" t="s">
-        <v>139</v>
+        <v>356</v>
       </c>
       <c r="D113" t="s">
-        <v>456</v>
+        <v>395</v>
       </c>
       <c r="E113" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+        <v>457</v>
+      </c>
+      <c r="F113" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>23</v>
-      </c>
-      <c r="B114" t="s">
-        <v>355</v>
+        <v>365</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>541</v>
       </c>
       <c r="C114" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="D114" t="s">
-        <v>457</v>
+        <v>364</v>
       </c>
       <c r="E114" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+        <v>458</v>
+      </c>
+      <c r="F114" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>24</v>
-      </c>
-      <c r="B115" t="s">
-        <v>356</v>
+        <v>30</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>542</v>
       </c>
       <c r="C115" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
       <c r="D115" t="s">
-        <v>458</v>
+        <v>369</v>
       </c>
       <c r="E115" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+        <v>459</v>
+      </c>
+      <c r="F115" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>365</v>
-      </c>
-      <c r="B116" t="s">
-        <v>363</v>
+        <v>31</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>543</v>
       </c>
       <c r="C116" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D116" t="s">
-        <v>459</v>
+        <v>370</v>
       </c>
       <c r="E116" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+        <v>460</v>
+      </c>
+      <c r="F116" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>30</v>
-      </c>
-      <c r="B117" t="s">
-        <v>367</v>
+        <v>32</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>544</v>
       </c>
       <c r="C117" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D117" t="s">
-        <v>460</v>
+        <v>372</v>
       </c>
       <c r="E117" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+      <c r="F117" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" t="s">
-        <v>368</v>
+        <v>34</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>545</v>
       </c>
       <c r="C118" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D118" t="s">
-        <v>461</v>
+        <v>375</v>
       </c>
       <c r="E118" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+        <v>462</v>
+      </c>
+      <c r="F118" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>32</v>
-      </c>
-      <c r="B119" t="s">
-        <v>371</v>
+        <v>35</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>546</v>
       </c>
       <c r="C119" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D119" t="s">
-        <v>462</v>
+        <v>376</v>
       </c>
       <c r="E119" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+      <c r="F119" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>34</v>
-      </c>
-      <c r="B120" t="s">
-        <v>373</v>
+        <v>36</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>547</v>
       </c>
       <c r="C120" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="D120" t="s">
-        <v>463</v>
+        <v>396</v>
       </c>
       <c r="E120" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+      <c r="F120" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>35</v>
-      </c>
-      <c r="B121" t="s">
-        <v>374</v>
+        <v>37</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>548</v>
       </c>
       <c r="C121" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="D121" t="s">
-        <v>464</v>
+        <v>397</v>
       </c>
       <c r="E121" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+        <v>465</v>
+      </c>
+      <c r="F121" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>36</v>
-      </c>
-      <c r="B122" t="s">
-        <v>383</v>
+        <v>385</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>549</v>
       </c>
       <c r="C122" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="D122" t="s">
-        <v>465</v>
+        <v>382</v>
       </c>
       <c r="E122" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+        <v>466</v>
+      </c>
+      <c r="F122" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>37</v>
-      </c>
-      <c r="B123" t="s">
-        <v>384</v>
+        <v>40</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>527</v>
       </c>
       <c r="C123" t="s">
-        <v>397</v>
-      </c>
-      <c r="D123" t="s">
-        <v>466</v>
-      </c>
-      <c r="E123" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>385</v>
-      </c>
-      <c r="B124" t="s">
-        <v>381</v>
+        <v>319</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>550</v>
       </c>
       <c r="C124" t="s">
-        <v>382</v>
+        <v>320</v>
       </c>
       <c r="D124" t="s">
-        <v>467</v>
-      </c>
-      <c r="E124" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>40</v>
-      </c>
-      <c r="B125" t="s">
-        <v>386</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
-        <v>319</v>
-      </c>
-      <c r="B126" t="s">
-        <v>320</v>
-      </c>
-      <c r="C126" t="s">
         <v>321</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated variable list and map titles
</commit_message>
<xml_diff>
--- a/data/NFHS Cascade Variable List.xlsx
+++ b/data/NFHS Cascade Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5611602-8257-4ED7-BA3B-6FAE88CD39EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A540E09-091F-4268-8D6D-804BA6714F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3244" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="1365">
   <si>
     <t>label</t>
   </si>
@@ -4492,10 +4492,10 @@
   <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G127" sqref="G127"/>
+      <selection pane="bottomRight" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4829,6 +4829,9 @@
         <v>479</v>
       </c>
       <c r="F17" t="s">
+        <v>479</v>
+      </c>
+      <c r="G17" t="s">
         <v>479</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added datasets for only eligible population
</commit_message>
<xml_diff>
--- a/data/NFHS Cascade Variable List.xlsx
+++ b/data/NFHS Cascade Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A540E09-091F-4268-8D6D-804BA6714F51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1481FB7-8416-4100-B336-D1292E3D691E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="1377">
   <si>
     <t>label</t>
   </si>
@@ -4123,6 +4123,42 @@
   </si>
   <si>
     <t>hv041</t>
+  </si>
+  <si>
+    <t>v006</t>
+  </si>
+  <si>
+    <t>v007</t>
+  </si>
+  <si>
+    <t>v016</t>
+  </si>
+  <si>
+    <t>v008</t>
+  </si>
+  <si>
+    <t>v008a</t>
+  </si>
+  <si>
+    <t>v009</t>
+  </si>
+  <si>
+    <t>mv006</t>
+  </si>
+  <si>
+    <t>mv007</t>
+  </si>
+  <si>
+    <t>mv016</t>
+  </si>
+  <si>
+    <t>mv008</t>
+  </si>
+  <si>
+    <t>mv008a</t>
+  </si>
+  <si>
+    <t>mv009</t>
   </si>
 </sst>
 </file>
@@ -4492,10 +4528,10 @@
   <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E121" sqref="E121"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4755,6 +4791,12 @@
       <c r="B12" t="s">
         <v>497</v>
       </c>
+      <c r="C12" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1371</v>
+      </c>
       <c r="E12" t="s">
         <v>475</v>
       </c>
@@ -4769,6 +4811,12 @@
       <c r="B13" t="s">
         <v>498</v>
       </c>
+      <c r="C13" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1372</v>
+      </c>
       <c r="E13" t="s">
         <v>476</v>
       </c>
@@ -4783,6 +4831,12 @@
       <c r="B14" t="s">
         <v>499</v>
       </c>
+      <c r="C14" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1373</v>
+      </c>
       <c r="E14" t="s">
         <v>487</v>
       </c>
@@ -4797,6 +4851,12 @@
       <c r="B15" t="s">
         <v>500</v>
       </c>
+      <c r="C15" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1374</v>
+      </c>
       <c r="E15" t="s">
         <v>477</v>
       </c>
@@ -4811,6 +4871,12 @@
       <c r="B16" t="s">
         <v>501</v>
       </c>
+      <c r="C16" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1375</v>
+      </c>
       <c r="E16" t="s">
         <v>478</v>
       </c>
@@ -4824,6 +4890,12 @@
       </c>
       <c r="B17" t="s">
         <v>502</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1376</v>
       </c>
       <c r="E17" t="s">
         <v>479</v>

</xml_diff>

<commit_message>
Commit after updating draft with figures and including youth diagnosed
</commit_message>
<xml_diff>
--- a/data/NFHS Cascade Variable List.xlsx
+++ b/data/NFHS Cascade Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6E10FE-F711-4EA3-8419-B5FE1148FBD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B612FA-951B-48B1-80D8-9D14AFA1559A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7a variables" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7474" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7476" uniqueCount="1480">
   <si>
     <t>label</t>
   </si>
@@ -4466,6 +4466,12 @@
   </si>
   <si>
     <t>Warangal</t>
+  </si>
+  <si>
+    <t>education of hh</t>
+  </si>
+  <si>
+    <t>educationhh</t>
   </si>
 </sst>
 </file>
@@ -4932,13 +4938,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BB052-C333-4DDF-AF33-13FC35516278}">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5387,1602 +5393,1610 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>313</v>
+        <v>1478</v>
       </c>
       <c r="B22" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C22" t="s">
-        <v>315</v>
-      </c>
-      <c r="D22" t="s">
-        <v>314</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B23" t="s">
-        <v>502</v>
+        <v>1406</v>
       </c>
       <c r="C23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D23" t="s">
-        <v>318</v>
-      </c>
-      <c r="E23" t="s">
-        <v>421</v>
-      </c>
-      <c r="F23" t="s">
-        <v>422</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>316</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
+        <v>502</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>317</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>318</v>
       </c>
       <c r="E24" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F24" t="s">
-        <v>290</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>313</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F25" t="s">
-        <v>419</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>492</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="E26" t="s">
+        <v>419</v>
+      </c>
+      <c r="F26" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>294</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C27" t="s">
-        <v>292</v>
+        <v>125</v>
       </c>
       <c r="D27" t="s">
-        <v>297</v>
-      </c>
-      <c r="E27" t="s">
-        <v>423</v>
-      </c>
-      <c r="F27" t="s">
-        <v>289</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B28" t="s">
-        <v>1393</v>
+        <v>503</v>
       </c>
       <c r="C28" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D28" t="s">
-        <v>293</v>
+        <v>297</v>
+      </c>
+      <c r="E28" t="s">
+        <v>423</v>
+      </c>
+      <c r="F28" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>295</v>
       </c>
       <c r="B29" t="s">
-        <v>504</v>
+        <v>1393</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>296</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" t="s">
-        <v>424</v>
-      </c>
-      <c r="F29" t="s">
-        <v>424</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F30" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>426</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>507</v>
+        <v>505</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
       </c>
       <c r="E31" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F31" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B32" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>429</v>
       </c>
       <c r="B33" t="s">
-        <v>552</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>154</v>
+        <v>506</v>
       </c>
       <c r="E33" t="s">
-        <v>557</v>
+        <v>428</v>
       </c>
       <c r="F33" t="s">
-        <v>557</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>553</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>554</v>
+        <v>552</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>154</v>
       </c>
       <c r="E34" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F34" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>553</v>
       </c>
       <c r="B35" t="s">
-        <v>555</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" t="s">
-        <v>159</v>
+        <v>554</v>
       </c>
       <c r="E35" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F35" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>564</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="C36" t="s">
-        <v>341</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>342</v>
+        <v>159</v>
       </c>
       <c r="E36" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F36" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>564</v>
       </c>
       <c r="B37" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>341</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>342</v>
       </c>
       <c r="E37" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F37" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>565</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="C38" t="s">
-        <v>343</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>344</v>
+        <v>160</v>
       </c>
       <c r="E38" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F38" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>565</v>
       </c>
       <c r="B39" t="s">
-        <v>1374</v>
+        <v>566</v>
       </c>
       <c r="C39" t="s">
-        <v>324</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="D39" t="s">
+        <v>344</v>
+      </c>
+      <c r="E39" t="s">
+        <v>561</v>
+      </c>
+      <c r="F39" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>358</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="C40" t="s">
-        <v>326</v>
-      </c>
-      <c r="D40" t="s">
-        <v>331</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>358</v>
       </c>
       <c r="B41" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="C41" t="s">
-        <v>325</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>326</v>
+      </c>
+      <c r="D41" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="C42" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>360</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="C43" t="s">
-        <v>334</v>
-      </c>
-      <c r="D43" t="s">
-        <v>335</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>360</v>
       </c>
       <c r="B44" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="C44" t="s">
-        <v>327</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E44" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="D44" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C45" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="C46" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>229</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>508</v>
+        <v>1381</v>
       </c>
       <c r="C47" t="s">
-        <v>249</v>
-      </c>
-      <c r="D47" t="s">
-        <v>239</v>
-      </c>
-      <c r="E47" t="s">
-        <v>484</v>
-      </c>
-      <c r="F47" t="s">
-        <v>484</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B48" t="s">
-        <v>1382</v>
+        <v>508</v>
       </c>
       <c r="C48" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D48" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+      <c r="E48" t="s">
+        <v>484</v>
+      </c>
+      <c r="F48" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B49" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B50" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="C50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B51" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B52" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B53" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="C53" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B54" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="C54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B55" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="C55" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B56" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C56" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D56" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>238</v>
       </c>
       <c r="B57" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>258</v>
+      </c>
+      <c r="D57" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>509</v>
+        <v>1392</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
-      </c>
-      <c r="E59" t="s">
-        <v>430</v>
-      </c>
-      <c r="F59" t="s">
-        <v>279</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B60" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E60" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>281</v>
+        <v>179</v>
       </c>
       <c r="B61" t="s">
-        <v>511</v>
+        <v>510</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
       </c>
       <c r="E61" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F61" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>281</v>
       </c>
       <c r="B62" t="s">
-        <v>512</v>
-      </c>
-      <c r="C62" t="s">
-        <v>68</v>
+        <v>511</v>
       </c>
       <c r="E62" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F62" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>388</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C63" t="s">
-        <v>389</v>
-      </c>
-      <c r="D63" t="s">
-        <v>403</v>
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>434</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G63" s="2"/>
+        <v>433</v>
+      </c>
+      <c r="F63" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B64" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C64" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D64" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E64" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>436</v>
+        <v>390</v>
       </c>
       <c r="B65" t="s">
-        <v>515</v>
+        <v>514</v>
+      </c>
+      <c r="C65" t="s">
+        <v>391</v>
+      </c>
+      <c r="D65" t="s">
+        <v>404</v>
       </c>
       <c r="E65" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B66" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E66" t="s">
-        <v>473</v>
+        <v>437</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>473</v>
+        <v>437</v>
       </c>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>181</v>
+        <v>438</v>
       </c>
       <c r="B67" t="s">
-        <v>517</v>
-      </c>
-      <c r="C67" t="s">
-        <v>182</v>
+        <v>516</v>
       </c>
       <c r="E67" t="s">
-        <v>440</v>
-      </c>
-      <c r="F67" t="s">
-        <v>285</v>
-      </c>
+        <v>473</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B68" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E69" t="s">
-        <v>442</v>
+        <v>441</v>
+      </c>
+      <c r="F69" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E70" t="s">
-        <v>443</v>
-      </c>
-      <c r="F70" t="s">
-        <v>287</v>
+        <v>442</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E71" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>446</v>
+        <v>187</v>
       </c>
       <c r="B72" t="s">
-        <v>522</v>
+        <v>521</v>
+      </c>
+      <c r="C72" t="s">
+        <v>190</v>
       </c>
       <c r="E72" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F72" t="s">
-        <v>447</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>271</v>
+        <v>446</v>
+      </c>
+      <c r="B73" t="s">
+        <v>522</v>
+      </c>
+      <c r="E73" t="s">
+        <v>445</v>
+      </c>
+      <c r="F73" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>272</v>
-      </c>
-      <c r="B74" t="s">
-        <v>495</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="D74" t="s">
-        <v>347</v>
-      </c>
-      <c r="E74" t="s">
-        <v>487</v>
-      </c>
-      <c r="F74" t="s">
-        <v>487</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>488</v>
+        <v>272</v>
       </c>
       <c r="B75" t="s">
-        <v>549</v>
-      </c>
-      <c r="C75" s="2"/>
+        <v>495</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D75" t="s">
+        <v>347</v>
+      </c>
       <c r="E75" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F75" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>270</v>
+        <v>488</v>
       </c>
       <c r="B76" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="D76" t="s">
-        <v>348</v>
+        <v>549</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="E76" t="s">
+        <v>489</v>
+      </c>
+      <c r="F76" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="B77" t="s">
-        <v>1394</v>
-      </c>
-      <c r="C77" t="s">
-        <v>210</v>
+        <v>1403</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>346</v>
       </c>
       <c r="D77" t="s">
-        <v>259</v>
+        <v>348</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B78" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="C78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B79" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="C79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D79" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B80" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B81" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="C81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D81" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B82" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B83" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="C83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B84" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="C84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D84" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B85" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="C85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B86" t="s">
-        <v>531</v>
+        <v>1402</v>
       </c>
       <c r="C86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D86" t="s">
-        <v>268</v>
-      </c>
-      <c r="E86" t="s">
-        <v>439</v>
-      </c>
-      <c r="F86" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>200</v>
+      </c>
+      <c r="B87" t="s">
+        <v>531</v>
+      </c>
+      <c r="C87" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" t="s">
+        <v>268</v>
+      </c>
+      <c r="E87" t="s">
+        <v>439</v>
+      </c>
+      <c r="F87" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>25</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>523</v>
-      </c>
-      <c r="C88" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="G88" s="5"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>1404</v>
+        <v>523</v>
       </c>
       <c r="C89" t="s">
-        <v>357</v>
+        <v>97</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>359</v>
+        <v>141</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>333</v>
+        <v>26</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>524</v>
+        <v>1404</v>
       </c>
       <c r="C90" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>333</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C91" t="s">
+        <v>361</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>400</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>401</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F92" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="s">
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>1405</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D93" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E93" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F93" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="G92" s="6"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>399</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="C93" t="s">
-        <v>378</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="G93" s="5"/>
+      <c r="G93" s="6"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>399</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C94" t="s">
-        <v>349</v>
-      </c>
-      <c r="D94" t="s">
-        <v>405</v>
-      </c>
-      <c r="E94" t="s">
-        <v>448</v>
-      </c>
-      <c r="F94" t="s">
-        <v>448</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C95" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D95" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E95" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F95" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C96" t="s">
+        <v>350</v>
+      </c>
+      <c r="D96" t="s">
+        <v>406</v>
+      </c>
+      <c r="E96" t="s">
+        <v>449</v>
+      </c>
+      <c r="F96" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>17</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>351</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>407</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E97" t="s">
         <v>450</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F97" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>18</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B98" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>352</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>408</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E98" t="s">
         <v>451</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F98" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>19</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>353</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>392</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E99" t="s">
         <v>452</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F99" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>20</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>354</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>393</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>453</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>366</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B101" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>95</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" t="s">
         <v>139</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E101" t="s">
         <v>454</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F101" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>23</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B102" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>355</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>394</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
         <v>455</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>24</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B103" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>356</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>395</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E103" t="s">
         <v>456</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F103" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>365</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>363</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>364</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E104" t="s">
         <v>457</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F104" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>30</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>367</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D105" t="s">
         <v>369</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
         <v>458</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F105" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>31</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B106" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>368</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D106" t="s">
         <v>370</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E106" t="s">
         <v>459</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F106" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>32</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>371</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
         <v>372</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E107" t="s">
         <v>460</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F107" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>34</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B108" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>373</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>375</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>461</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F108" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>35</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B109" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>374</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" t="s">
         <v>376</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
         <v>462</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F109" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>36</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B110" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>383</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D110" t="s">
         <v>396</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E110" t="s">
         <v>463</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F110" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B111" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>384</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D111" t="s">
         <v>397</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E111" t="s">
         <v>464</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F111" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>385</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>381</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>382</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E112" t="s">
         <v>465</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F112" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>40</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="C112" t="s">
-        <v>386</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G112" s="2"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>319</v>
+        <v>40</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
       <c r="C113" t="s">
-        <v>320</v>
-      </c>
-      <c r="D113" t="s">
-        <v>321</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B114" s="7"/>
-      <c r="G114" t="s">
-        <v>1358</v>
+        <v>319</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="C114" t="s">
+        <v>320</v>
+      </c>
+      <c r="D114" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="B115" s="7"/>
       <c r="G115" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B116" s="7"/>
+      <c r="G116" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>1356</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G117" t="s">
         <v>1361</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B39:B46">
+  <conditionalFormatting sqref="B40:B47">
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47:B55">
+  <conditionalFormatting sqref="B48:B56">
     <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B57">
+  <conditionalFormatting sqref="B57:B58">
     <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
+  <conditionalFormatting sqref="B59">
     <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
+  <conditionalFormatting sqref="B29">
     <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77:B86">
+  <conditionalFormatting sqref="B78:B87">
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76">
+  <conditionalFormatting sqref="B77">
     <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88:B93">
+  <conditionalFormatting sqref="B89:B94">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23733,8 +23747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66008B8-76F2-41E7-9777-62AFF2799EE5}">
   <dimension ref="A1:F641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changed map references to india shapefiles Added nfhs5 iapr_pregnant and nfhs5 iair pregnant
</commit_message>
<xml_diff>
--- a/data/NFHS Cascade Variable List.xlsx
+++ b/data/NFHS Cascade Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B612FA-951B-48B1-80D8-9D14AFA1559A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2B2F51-B2E6-4579-925D-37C322A1CDBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7a variables" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7476" uniqueCount="1480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7477" uniqueCount="1480">
   <si>
     <t>label</t>
   </si>
@@ -4940,7 +4940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BB052-C333-4DDF-AF33-13FC35516278}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8229,7 +8229,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8536,10 +8536,10 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -8550,10 +8550,10 @@
         <v>14</v>
       </c>
       <c r="C23">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -8564,10 +8564,10 @@
         <v>17</v>
       </c>
       <c r="C24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -8578,10 +8578,10 @@
         <v>15</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -8592,10 +8592,10 @@
         <v>23</v>
       </c>
       <c r="C26">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -8776,16 +8776,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7312AFEF-E9E5-4C74-901A-211FCC52E64C}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8794,10 +8794,10 @@
         <v>603</v>
       </c>
       <c r="B1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" t="s">
         <v>1456</v>
-      </c>
-      <c r="C1" t="s">
-        <v>308</v>
       </c>
       <c r="D1" t="s">
         <v>1455</v>
@@ -8811,10 +8811,10 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>600</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -8825,7 +8825,7 @@
         <v>28</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>593</v>
@@ -8839,7 +8839,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>578</v>
@@ -8853,7 +8853,7 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>584</v>
@@ -8867,7 +8867,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>576</v>
@@ -8881,7 +8881,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>570</v>
@@ -8895,7 +8895,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>588</v>
@@ -8905,405 +8905,413 @@
       <c r="A9" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>25</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="B10" s="8">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>573</v>
-      </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
       <c r="C10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>595</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="B11">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>590</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>572</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>602</v>
+        <v>567</v>
       </c>
       <c r="B16">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>594</v>
+        <v>567</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="B17">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>597</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="B18">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B19">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B20">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C21">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B22">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>573</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="B27">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="B28">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B31">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>598</v>
+        <v>577</v>
       </c>
       <c r="B32">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>598</v>
+        <v>577</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B33">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="B34">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>571</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>585</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>19</v>
       </c>
-      <c r="C37">
-        <v>19</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
         <v>585</v>
       </c>
     </row>
@@ -36587,7 +36595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6368BC-6D9A-4FE2-8E94-2948D2AC483C}">
   <dimension ref="A1:F708"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>